<commit_message>
clean up document name
</commit_message>
<xml_diff>
--- a/Projekt-Steuerung_Autonom-Fahrendes-Auto_Moftah.xlsx
+++ b/Projekt-Steuerung_Autonom-Fahrendes-Auto_Moftah.xlsx
@@ -1,66 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Matura\ESY\Ferngesteuertes_Auto_Moftah_Sakip\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Matura\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D25302A-A75E-4921-BB91-070F6C16D4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4F1408-7303-4806-8829-849EC65A508C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="31" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="63" activeTab="66" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="11" r:id="rId2"/>
-    <sheet name="Tabelle2" sheetId="12" r:id="rId3"/>
-    <sheet name="Tabelle3" sheetId="13" r:id="rId4"/>
-    <sheet name="Tabelle4" sheetId="14" r:id="rId5"/>
-    <sheet name="Tabelle5" sheetId="15" r:id="rId6"/>
-    <sheet name="Anforderungen" sheetId="2" r:id="rId7"/>
-    <sheet name="Meilensteine" sheetId="3" r:id="rId8"/>
-    <sheet name="Bestellliste" sheetId="4" r:id="rId9"/>
-    <sheet name="PSP - WBS" sheetId="5" r:id="rId10"/>
-    <sheet name="Tabelle6" sheetId="16" r:id="rId11"/>
-    <sheet name="Tabelle7" sheetId="17" r:id="rId12"/>
-    <sheet name="Tabelle8" sheetId="18" r:id="rId13"/>
-    <sheet name="Tabelle9" sheetId="19" r:id="rId14"/>
-    <sheet name="Tabelle10" sheetId="20" r:id="rId15"/>
-    <sheet name="Tabelle11" sheetId="21" r:id="rId16"/>
-    <sheet name="Tabelle12" sheetId="22" r:id="rId17"/>
-    <sheet name="Tabelle13" sheetId="23" r:id="rId18"/>
-    <sheet name="Tabelle14" sheetId="24" r:id="rId19"/>
-    <sheet name="Tabelle15" sheetId="25" r:id="rId20"/>
-    <sheet name="Tabelle16" sheetId="26" r:id="rId21"/>
-    <sheet name="Tabelle17" sheetId="27" r:id="rId22"/>
-    <sheet name="Tabelle18" sheetId="28" r:id="rId23"/>
-    <sheet name="Tabelle19" sheetId="29" r:id="rId24"/>
-    <sheet name="Tabelle20" sheetId="30" r:id="rId25"/>
-    <sheet name="Tabelle21" sheetId="31" r:id="rId26"/>
-    <sheet name="Tabelle22" sheetId="32" r:id="rId27"/>
-    <sheet name="Tabelle23" sheetId="33" r:id="rId28"/>
-    <sheet name="Tabelle24" sheetId="34" r:id="rId29"/>
-    <sheet name="OPL" sheetId="6" r:id="rId30"/>
-    <sheet name="Risiken" sheetId="7" r:id="rId31"/>
-    <sheet name="Stakeholder - Kommunikation" sheetId="8" r:id="rId32"/>
-    <sheet name="Arbeitstagebuch_Name" sheetId="9" r:id="rId33"/>
-    <sheet name="_Template" sheetId="10" r:id="rId34"/>
+    <sheet name="Anforderungen" sheetId="2" r:id="rId2"/>
+    <sheet name="Meilensteine" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabelle47" sheetId="63" r:id="rId4"/>
+    <sheet name="Tabelle48" sheetId="64" r:id="rId5"/>
+    <sheet name="Tabelle49" sheetId="65" r:id="rId6"/>
+    <sheet name="Tabelle50" sheetId="66" r:id="rId7"/>
+    <sheet name="Tabelle51" sheetId="67" r:id="rId8"/>
+    <sheet name="Tabelle52" sheetId="68" r:id="rId9"/>
+    <sheet name="Tabelle53" sheetId="69" r:id="rId10"/>
+    <sheet name="Tabelle54" sheetId="70" r:id="rId11"/>
+    <sheet name="Tabelle55" sheetId="71" r:id="rId12"/>
+    <sheet name="Tabelle56" sheetId="72" r:id="rId13"/>
+    <sheet name="Tabelle57" sheetId="73" r:id="rId14"/>
+    <sheet name="Tabelle58" sheetId="74" r:id="rId15"/>
+    <sheet name="Tabelle59" sheetId="75" r:id="rId16"/>
+    <sheet name="Tabelle60" sheetId="76" r:id="rId17"/>
+    <sheet name="Tabelle61" sheetId="77" r:id="rId18"/>
+    <sheet name="Tabelle62" sheetId="78" r:id="rId19"/>
+    <sheet name="Tabelle63" sheetId="79" r:id="rId20"/>
+    <sheet name="Tabelle64" sheetId="80" r:id="rId21"/>
+    <sheet name="Tabelle65" sheetId="81" r:id="rId22"/>
+    <sheet name="Tabelle66" sheetId="82" r:id="rId23"/>
+    <sheet name="Tabelle67" sheetId="83" r:id="rId24"/>
+    <sheet name="Tabelle68" sheetId="84" r:id="rId25"/>
+    <sheet name="Tabelle69" sheetId="85" r:id="rId26"/>
+    <sheet name="Tabelle70" sheetId="86" r:id="rId27"/>
+    <sheet name="Tabelle71" sheetId="87" r:id="rId28"/>
+    <sheet name="Bestellliste" sheetId="4" r:id="rId29"/>
+    <sheet name="PSP - WBS" sheetId="5" r:id="rId30"/>
+    <sheet name="Tabelle46" sheetId="62" r:id="rId31"/>
+    <sheet name="Tabelle1" sheetId="35" r:id="rId32"/>
+    <sheet name="Tabelle2" sheetId="36" r:id="rId33"/>
+    <sheet name="Tabelle3" sheetId="37" r:id="rId34"/>
+    <sheet name="Tabelle4" sheetId="38" r:id="rId35"/>
+    <sheet name="Tabelle5" sheetId="39" r:id="rId36"/>
+    <sheet name="Tabelle24" sheetId="40" r:id="rId37"/>
+    <sheet name="Tabelle25" sheetId="41" r:id="rId38"/>
+    <sheet name="Tabelle26" sheetId="42" r:id="rId39"/>
+    <sheet name="Tabelle27" sheetId="43" r:id="rId40"/>
+    <sheet name="Tabelle28" sheetId="44" r:id="rId41"/>
+    <sheet name="Tabelle29" sheetId="45" r:id="rId42"/>
+    <sheet name="Tabelle30" sheetId="46" r:id="rId43"/>
+    <sheet name="Tabelle31" sheetId="47" r:id="rId44"/>
+    <sheet name="Tabelle32" sheetId="48" r:id="rId45"/>
+    <sheet name="Tabelle33" sheetId="49" r:id="rId46"/>
+    <sheet name="Tabelle34" sheetId="50" r:id="rId47"/>
+    <sheet name="Tabelle35" sheetId="51" r:id="rId48"/>
+    <sheet name="Tabelle36" sheetId="52" r:id="rId49"/>
+    <sheet name="Tabelle37" sheetId="53" r:id="rId50"/>
+    <sheet name="Tabelle38" sheetId="54" r:id="rId51"/>
+    <sheet name="Tabelle39" sheetId="55" r:id="rId52"/>
+    <sheet name="Tabelle40" sheetId="56" r:id="rId53"/>
+    <sheet name="Tabelle41" sheetId="57" r:id="rId54"/>
+    <sheet name="Tabelle42" sheetId="58" r:id="rId55"/>
+    <sheet name="Tabelle43" sheetId="59" r:id="rId56"/>
+    <sheet name="Tabelle44" sheetId="60" r:id="rId57"/>
+    <sheet name="Tabelle45" sheetId="61" r:id="rId58"/>
+    <sheet name="Tabelle6" sheetId="16" r:id="rId59"/>
+    <sheet name="Tabelle7" sheetId="17" r:id="rId60"/>
+    <sheet name="Tabelle8" sheetId="18" r:id="rId61"/>
+    <sheet name="Tabelle9" sheetId="19" r:id="rId62"/>
+    <sheet name="Tabelle12" sheetId="22" r:id="rId63"/>
+    <sheet name="OPL" sheetId="6" r:id="rId64"/>
+    <sheet name="Risiken" sheetId="7" r:id="rId65"/>
+    <sheet name="Stakeholder - Kommunikation" sheetId="8" r:id="rId66"/>
+    <sheet name="Arbeitstagebuch_Name" sheetId="9" r:id="rId67"/>
+    <sheet name="_Template" sheetId="10" r:id="rId68"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId35"/>
+    <externalReference r:id="rId69"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'PSP - WBS'!$A$3:$I$7</definedName>
-    <definedName name="_ftnref1" localSheetId="9">'PSP - WBS'!$C$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="29" hidden="1">'PSP - WBS'!$A$3:$I$7</definedName>
+    <definedName name="_ftnref1" localSheetId="29">'PSP - WBS'!$C$3</definedName>
     <definedName name="Arbeitspaket">[1]Stammdaten!$A$9:$A$10</definedName>
     <definedName name="Personen">[1]Stammdaten!$A$27:$A$28</definedName>
     <definedName name="Prio">[1]Stammdaten!$A$16:$A$18</definedName>
     <definedName name="Status">[1]Stammdaten!$A$21:$A$24</definedName>
-    <definedName name="Text11" localSheetId="9">'PSP - WBS'!$C$11</definedName>
-    <definedName name="Text12" localSheetId="9">'PSP - WBS'!$B$11</definedName>
-    <definedName name="Text13" localSheetId="9">'PSP - WBS'!$B$18</definedName>
+    <definedName name="Text11" localSheetId="29">'PSP - WBS'!$C$11</definedName>
+    <definedName name="Text12" localSheetId="29">'PSP - WBS'!$B$11</definedName>
+    <definedName name="Text13" localSheetId="29">'PSP - WBS'!$B$18</definedName>
     <definedName name="Themen">[1]Stammdaten!$A$13</definedName>
     <definedName name="Typ">[1]Stammdaten!$A$4:$A$6</definedName>
   </definedNames>
@@ -288,7 +322,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="233">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -818,9 +852,6 @@
     <t>Implementierung Seitenregelung (inkl. Konfigurationsmöglichkeiten)</t>
   </si>
   <si>
-    <t>Implementierung Mittenregelung (inkl. Konfigurationsmöglichkeiten)</t>
-  </si>
-  <si>
     <t>Konzept für Drehzahlmessung pro Motor überlegen</t>
   </si>
   <si>
@@ -1112,9 +1143,6 @@
     <t>Inbetriebnahme der Infrarotsensoren / Ultraschallsensoren durch leicht verwendbares Interface zur Auswertung (generisch und effizient programmiert)</t>
   </si>
   <si>
-    <t>Arbeitstagebuch &lt;Name&gt;</t>
-  </si>
-  <si>
     <t>Sakip Gujlbear, Moftah Osama</t>
   </si>
   <si>
@@ -1143,6 +1171,39 @@
   </si>
   <si>
     <t>Weiter mit den Infrarotsensoren gearbeitet, Verbindung auf den Arduino Shield V5 verbunden, Code programmiert für die Infrarotsensoren, funktioniert, jedoch muss noch die Dinstanz nochmal überprüft werden, wie weit die Reichweite ist. Allerdings, druch den Test des Codes, fuhr das Auto in einer Wand, Infrarot dadurch abgefallen und die Draht-Verbindung wurden ausgesteckt, Danach nochmal ausgelötet , die Verbindung von neu gemacht, allerdings ist der Infrarot verbrannt worden. Müssen jetzt warten bis welche kommen. Partner mit Taster  geholfen und versucht den Fehler zu finden beim Code und der Hardware. Wenn die Infrarot Sensoren nicht nächstes Mal kommen, wird der Ultraschallsensor ausgetestet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es wurde letzte Woche besprochen, dass wir die Stunden vom 11.12.23 verwenden werden, um Github herunterzuladen. Am Anfang der Stunde gab eine Einführung und zwar was genau Github ist und wozu dient es. Am wichtigsten zu merken war, man verwendet Github, um mit dem Partner gleichzeitig auf einem Programm arbeiten zu können. Nach der Einführung begannen wir Sourcetree und Github herunterzuladen. Nachdem es erfolgreich auf dem Laptop hochgeladen wurde, wurde drauf experemtiert, um zu verstehen wie es in Sourcetree funktioniert. Als Beispiel sollte man eine Sache bearbeiten in der Readme Datei. Wichtig zu beachten!! Es haben zwei gleichzeitig drauf gearbeitet und die Readme Dataei geändert. Allerdings, derjenige der als erstes fertig war mit der Änderung und es commitet hat, war fertig und musste nichts mehr machen. Jedoch die Person, die erst später fertig geworden ist, musste den Teil vom ersten Partner mit seinem Teil, welches er auch verändert hat, zusammenfügen und dann commiten. Dann würde es funktionieren. Es erscheint dann ein sogenannter Graph.  Danach wurde weiter auf dem Ultraschall Sensor gearbeitet, da noch nicht die Infrarot Sensoren gekommen sind. Unötige verkaplungen ausgelötet, dann richtige Verkablung verbunden auf dem Arduino Shield V5 und den Sensoren eingeschraubt. </t>
+  </si>
+  <si>
+    <t>Arbeitstagebuch Moftah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problem mit Github gehabt am Anfang der Stunde. Danach neue Sensoren (Infrarot Sensoren) angekommen. Sensoren: Drähte abisoliert verbunden mit den Sensoren, Verkablungen auf die richtigen Anschlüsse verbunden, Kabelschlauch extra verwendet, um es zu befestigen. Danach die Sensoren auf dem Auto eingeschraubt, jedoch wurde als erstes der kleine Sensor eingeschraubt, um zu testen, ob er funktioniert mit dem Code, welches programmiert wurde. Es hat funktioniert und er stoppte, weil der Sensor eine Wand erkannt hat. Der 2te kleine Sensor konnte nicht eingeschraubt werden, da die Befestgiung letztens kaputt ging. Es wurde dann eins ausgedruckt (3D-Drucker). Beim größeren Infrarot Sensor gab es das Problem, dass das Auto keine guten Durchbohrung hat auf dem Auto, dass der Sensor in Sicherheit ist, wenn er gegen eine Sache fährt. Daher wurde beschlossen, ein extra Loch in der Mitte zu bohren. Trotz des fehlendes Loches, wurde der großere Sensor irgendwo eingeschraubt, um ihn zu testen, ober funktioniert oder vielleicht durchgebrannt ist. Ein Code wurde dann von mir und  meinem Partner geschrieben, der Sensor funktioniert. Es wurde dann die Seitenreglung ausprobiert. Es hat funktioniert, jedoch reagiert der großere Sensor zu langsam als der kleinere Sensor. Anders gesagt: Das Auto fährt und wenn es eine Wand erkennt, fährt es als in die Wand und dann biegt  es erst. Mein Partner und ich versuchten den Fehler zu finden, er wurde leider noch nicht behoben, aber beim nächsten Mal. </t>
+  </si>
+  <si>
+    <t>Wir hatten diesmal nur 2h, da wir anstatt 3h DIC, hatten wir 4h. In der 1h zeigte uns der Professor eine Übersicht, wie ein sauberes Program bezüglich des Projekt aussehen sollte und man es einfach machen könnte. Während sein Vortrags, zeichnete er auf der Tafel, wie eigentlich das Auto startet,stoppt, Vorwärts und Rückwärtsfährt fährt und was genau die Aufgabe ist der Sensoren wenn das Auto fährt. Nachdem Vortrag, wurde ein Meilenstein augesetzt, und zwar soll bis zum 15.01.24 stabile Messwerte der Sensoren ausgeben werden. In der 2h wurde der letzte Sensor auf dem Auto eingeschraubt. Anschließend wurde ein Code mit meinem Partner geschrieben, der alle 3 Sensoren zum Testen gebracht hatte. Jedoch haben am Ende nur 2 Sensoren funktioniert, der linke und der in der Mitte haben funktioniert. Der Rechte hat nicht reagiert, wenn eine Wand vor ihn kam, er ist gegen die Wand gefahren, jedoch die anderen 2 nicht. Der in der Mitte hat reagiert wenn eine Wand vor ihn ist und der linke ebenso. Es wurden dann die Pins umgetauscht, zum Beispiel, wenn der linke Sensor A0 war und der Rechte A1, haben wir die Pins getauscht und aufeinmal ging der Rechte Sensor zu reagieren und der linke nicht mehr.  Es gibt höchstwahrscheinlich einige Fehler im Code, jedoch konnten wir in dieser Stunde den Fehler nicht beheben.</t>
+  </si>
+  <si>
+    <t>Wurde erfolgreich gewählt, 3 Infrarotsensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hat länger gedauert, da die Sensor erst später kamen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kleine Code programmiert, um zu testen </t>
+  </si>
+  <si>
+    <t>Implementierung Mittenreglung(inkl. Konfigurationsmöglichkeiten)</t>
+  </si>
+  <si>
+    <t>Noch nicht drauf gearbeitet</t>
+  </si>
+  <si>
+    <t>Entschieden für Mittenregelung</t>
+  </si>
+  <si>
+    <t>Es wurde das Vorwärts, Rechts-Erkennung, Links-Erkennung, Rückwärts fahren auf der Rennstrecke überprüft. Jedoch war es nicht erfolgreich, wie geplant. Es wurde ein Code programmiert mit meinem Partner, der allerdings funktioniert, jedoch ist die Formel für die Differenz nicht genau und es sollte bis zum nächsten Mal eine Formel gefunden werden, die in cm umrechnet, da es präziser ist. Ein weiter Fehler war die Geschwindigkeit, Seine maximale Geschwindigkeit sollte eigentlch bei Vorwärts fahren und nicht beim rechts abbiegen. Die muss ebenso beim nächsten Mal verändert werden. Bezüglich den stabillen Messungen der Sensoren war es nicht genau, es hatte einen Unterschied von ca 40(keine cm!)</t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1603,7 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1854,6 +1915,30 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1872,33 +1957,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1922,6 +1983,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2092,9 +2156,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2132,7 +2196,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2238,7 +2302,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2380,7 +2444,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2393,7 +2457,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ29"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="112" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="112" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2408,14 +2472,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="118" t="s">
-        <v>204</v>
-      </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
+      <c r="A1" s="107" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -2464,22 +2528,22 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="113" t="s">
+      <c r="E7" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="113"/>
+      <c r="F7" s="108"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2488,8 +2552,8 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="110"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
@@ -2498,8 +2562,8 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="121"/>
-      <c r="F10" s="121"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="111"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2508,8 +2572,8 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="112"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="17"/>
@@ -2530,49 +2594,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="116"/>
-      <c r="C15" s="116"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
-      <c r="F15" s="116"/>
+      <c r="B15" s="113"/>
+      <c r="C15" s="113"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="114"/>
+      <c r="E16" s="114"/>
+      <c r="F16" s="114"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="117"/>
-      <c r="C17" s="117"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="114"/>
+      <c r="D17" s="114"/>
+      <c r="E17" s="114"/>
+      <c r="F17" s="114"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="117"/>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
+      <c r="B18" s="114"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="114"/>
+      <c r="E18" s="114"/>
+      <c r="F18" s="114"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="111"/>
-      <c r="C19" s="111"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="111"/>
+      <c r="B19" s="119"/>
+      <c r="C19" s="119"/>
+      <c r="D19" s="119"/>
+      <c r="E19" s="119"/>
+      <c r="F19" s="119"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
@@ -2585,74 +2649,64 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="112" t="s">
+      <c r="A23" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="112"/>
-      <c r="C23" s="112"/>
-      <c r="D23" s="112"/>
-      <c r="E23" s="112"/>
-      <c r="F23" s="112"/>
+      <c r="B23" s="120"/>
+      <c r="C23" s="120"/>
+      <c r="D23" s="120"/>
+      <c r="E23" s="120"/>
+      <c r="F23" s="120"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="113" t="s">
+      <c r="A26" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="113"/>
-      <c r="C26" s="113"/>
-      <c r="D26" s="113" t="s">
+      <c r="B26" s="108"/>
+      <c r="C26" s="108"/>
+      <c r="D26" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="113"/>
-      <c r="F26" s="113"/>
+      <c r="E26" s="108"/>
+      <c r="F26" s="108"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="108" t="s">
+      <c r="A27" s="116" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="108"/>
-      <c r="C27" s="108"/>
-      <c r="D27" s="114"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="114"/>
+      <c r="B27" s="116"/>
+      <c r="C27" s="116"/>
+      <c r="D27" s="121"/>
+      <c r="E27" s="121"/>
+      <c r="F27" s="121"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="107" t="s">
+      <c r="A28" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="107"/>
-      <c r="C28" s="107"/>
-      <c r="D28" s="108" t="s">
-        <v>205</v>
-      </c>
-      <c r="E28" s="108"/>
-      <c r="F28" s="108"/>
+      <c r="B28" s="115"/>
+      <c r="C28" s="115"/>
+      <c r="D28" s="116" t="s">
+        <v>204</v>
+      </c>
+      <c r="E28" s="116"/>
+      <c r="F28" s="116"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="109" t="s">
+      <c r="A29" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="109"/>
-      <c r="C29" s="109"/>
-      <c r="D29" s="110"/>
-      <c r="E29" s="110"/>
-      <c r="F29" s="110"/>
+      <c r="B29" s="117"/>
+      <c r="C29" s="117"/>
+      <c r="D29" s="118"/>
+      <c r="E29" s="118"/>
+      <c r="F29" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2663,6 +2717,16 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2671,14 +2735,1085 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F53BD46-419E-42C4-A71A-0B25B0882ACB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4910CDE0-C825-466D-91FA-B7598033BFE1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B94CA25-6AC6-465E-B913-A90B002B4FC3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCF8EFB-7803-4589-8BE5-A46D8D977B1F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FFFFD96-6DA9-41A8-8062-691D3E820DC6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA962B70-5DE7-4C26-A5B4-43564547E906}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE57E93-9F45-44F0-83D2-9BE417AB37BB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35761FCD-184C-494C-BB43-361D1928B764}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9420BC3C-F9F7-4CE7-BDA7-10C2C1A0518F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D741A5E-0A64-4270-8A80-589507A65A1E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" zoomScale="84" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.109375" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" style="25" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="64" width="10.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="107" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+    </row>
+    <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="122" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="122"/>
+    </row>
+    <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="122" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="122"/>
+    </row>
+    <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="122" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="122"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="28">
+        <v>10</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="30"/>
+    </row>
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="28">
+        <v>20</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10" s="30"/>
+    </row>
+    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="28">
+        <v>30</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="30"/>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="28">
+        <v>40</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="30"/>
+    </row>
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="28">
+        <v>51</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="30"/>
+    </row>
+    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="28">
+        <v>52</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="30"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="28">
+        <v>60</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="30"/>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="28">
+        <v>61</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="30"/>
+    </row>
+    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="28">
+        <v>62</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="30"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="28">
+        <v>50</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="28">
+        <v>60</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="28">
+        <v>70</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="28">
+        <v>80</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="28">
+        <v>90</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="28">
+        <v>100</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="32">
+        <v>110</v>
+      </c>
+      <c r="B25" s="33"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E436902-616E-4673-899A-23819F5DA605}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66F03A7-ED43-43CE-B704-FB3FB0C9410F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D20D7C-7922-4517-846E-0401E1B1D7AA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A44D925B-8160-4690-A689-9800AEAA65AE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFA43E2-62CA-4B5C-B9AA-697D8FD95677}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711D2D94-E2C9-4782-B583-81102FA23CB0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDFDCEB-E741-4288-AC2E-3B7261C1B994}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5684BEB-D1CD-4600-8730-AA30690C5F7D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2465DF68-317D-4286-8194-2DC472CD9B01}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ21"/>
+  <sheetViews>
+    <sheetView zoomScale="87" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.44140625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" style="23" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" style="35" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="68.6640625" style="23" customWidth="1"/>
+    <col min="7" max="1024" width="11.44140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="123" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+    </row>
+    <row r="3" spans="1:6" s="43" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="41">
+        <v>1</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="41">
+        <v>1</v>
+      </c>
+      <c r="D4" s="44">
+        <v>50</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="41">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="41">
+        <v>2</v>
+      </c>
+      <c r="D5" s="44">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="41">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="41">
+        <v>1</v>
+      </c>
+      <c r="D6" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="45"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="41">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="41">
+        <v>1</v>
+      </c>
+      <c r="D7" s="44">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="41">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="44">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="41">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="41">
+        <v>1</v>
+      </c>
+      <c r="D9" s="44">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="41">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="41">
+        <v>1</v>
+      </c>
+      <c r="D10" s="44">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="41">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="41">
+        <v>3</v>
+      </c>
+      <c r="D11" s="44">
+        <v>45</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="46"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="41">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="41">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="41">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="41">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="41">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="41">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="41">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="41">
+        <v>29</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="42">
+        <v>30</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+    </row>
+    <row r="21" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="47"/>
+      <c r="B21" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="47"/>
+      <c r="D21" s="48">
+        <f>SUM(D4:D20)</f>
+        <v>121.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="F5" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:C41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="114" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="56.44140625" customWidth="1"/>
+    <col min="2" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="64" width="10.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="123" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="23"/>
+    </row>
+    <row r="3" spans="1:3" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="124" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+    </row>
+    <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="125" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="23"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="37">
+        <v>45236</v>
+      </c>
+      <c r="C7" s="37">
+        <v>45236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="39">
+        <v>45243</v>
+      </c>
+      <c r="C8" s="39">
+        <v>45257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="38" t="s">
+        <v>208</v>
+      </c>
+      <c r="B9" s="39">
+        <v>45257</v>
+      </c>
+      <c r="C9" s="39">
+        <v>45264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="40">
+        <v>45271</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="39">
+        <v>45278</v>
+      </c>
+      <c r="C11" s="40">
+        <v>44941</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="39">
+        <v>45306</v>
+      </c>
+      <c r="C12" s="41"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="39">
+        <v>45320</v>
+      </c>
+      <c r="C13" s="41"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="39">
+        <v>45341</v>
+      </c>
+      <c r="C14" s="41"/>
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="39">
+        <v>45355</v>
+      </c>
+      <c r="C15" s="41"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="39">
+        <v>45362</v>
+      </c>
+      <c r="C16" s="41"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="41"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="2"/>
+      <c r="B40" s="41"/>
+      <c r="C40" s="41"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="24"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="74" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2692,16 +3827,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="107" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
     </row>
     <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -2788,7 +3923,7 @@
         <v>45236</v>
       </c>
       <c r="I6" s="59" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
@@ -2869,7 +4004,7 @@
         <v>102</v>
       </c>
       <c r="C11" s="56" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D11" s="57">
         <v>2</v>
@@ -2888,7 +4023,7 @@
         <v>103</v>
       </c>
       <c r="C12" s="56" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D12" s="57">
         <v>2</v>
@@ -2907,7 +4042,7 @@
         <v>104</v>
       </c>
       <c r="C13" s="56" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D13" s="57">
         <v>3</v>
@@ -2926,7 +4061,7 @@
         <v>105</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D14" s="57">
         <v>1</v>
@@ -2968,40 +4103,60 @@
         <v>31</v>
       </c>
       <c r="B17" s="55" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C17" s="56" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D17" s="57">
         <v>2</v>
       </c>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="59"/>
-    </row>
-    <row r="18" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="E17" s="56">
+        <v>1</v>
+      </c>
+      <c r="F17" s="56">
+        <v>0</v>
+      </c>
+      <c r="G17" s="58">
+        <v>45248</v>
+      </c>
+      <c r="H17" s="58">
+        <v>45255</v>
+      </c>
+      <c r="I17" s="59" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
         <v>32</v>
       </c>
       <c r="B18" s="55" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C18" s="56" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D18" s="57">
         <v>3</v>
       </c>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="59"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E18" s="56">
+        <v>8</v>
+      </c>
+      <c r="F18" s="56">
+        <v>0</v>
+      </c>
+      <c r="G18" s="58">
+        <v>45264</v>
+      </c>
+      <c r="H18" s="58">
+        <v>45278</v>
+      </c>
+      <c r="I18" s="59" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A19" s="28">
         <v>34</v>
       </c>
@@ -3009,16 +4164,26 @@
         <v>107</v>
       </c>
       <c r="C19" s="56" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D19" s="57">
         <v>3</v>
       </c>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="59"/>
+      <c r="E19" s="56">
+        <v>2</v>
+      </c>
+      <c r="F19" s="56">
+        <v>0</v>
+      </c>
+      <c r="G19" s="58">
+        <v>45255</v>
+      </c>
+      <c r="H19" s="58">
+        <v>45255</v>
+      </c>
+      <c r="I19" s="59" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
@@ -3029,7 +4194,7 @@
       </c>
       <c r="C20" s="106"/>
       <c r="D20" s="62" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E20" s="56"/>
       <c r="F20" s="56"/>
@@ -3071,7 +4236,7 @@
         <v>110</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D23" s="64">
         <v>10</v>
@@ -3090,16 +4255,20 @@
         <v>111</v>
       </c>
       <c r="C24" s="56" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D24" s="64">
         <v>10</v>
       </c>
-      <c r="E24" s="65"/>
+      <c r="E24" s="65" t="s">
+        <v>216</v>
+      </c>
       <c r="F24" s="65"/>
       <c r="G24" s="58"/>
       <c r="H24" s="65"/>
-      <c r="I24" s="66"/>
+      <c r="I24" s="66" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="63">
@@ -3109,7 +4278,7 @@
         <v>112</v>
       </c>
       <c r="C25" s="56" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D25" s="64">
         <v>10</v>
@@ -3128,26 +4297,36 @@
         <v>113</v>
       </c>
       <c r="C26" s="56" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D26" s="64">
         <v>10</v>
       </c>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="66"/>
+      <c r="E26" s="65">
+        <v>3</v>
+      </c>
+      <c r="F26" s="65">
+        <v>0</v>
+      </c>
+      <c r="G26" s="58">
+        <v>45271</v>
+      </c>
+      <c r="H26" s="130">
+        <v>45279</v>
+      </c>
+      <c r="I26" s="66" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="63">
         <v>45</v>
       </c>
       <c r="B27" s="67" t="s">
-        <v>114</v>
+        <v>229</v>
       </c>
       <c r="C27" s="56" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D27" s="64">
         <v>10</v>
@@ -3163,10 +4342,10 @@
         <v>46</v>
       </c>
       <c r="B28" s="67" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C28" s="61" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D28" s="68">
         <v>10</v>
@@ -3182,10 +4361,10 @@
         <v>47</v>
       </c>
       <c r="B29" s="55" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C29" s="61" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D29" s="62">
         <v>10</v>
@@ -3201,10 +4380,10 @@
         <v>48</v>
       </c>
       <c r="B30" s="55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C30" s="61" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D30" s="62">
         <v>11</v>
@@ -3266,7 +4445,7 @@
       </c>
       <c r="E35" s="49">
         <f>SUM(E10:E34)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F35" s="49">
         <f>SUM(F10:F34)</f>
@@ -3288,7 +4467,367 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8819D0AD-0B9B-4F12-A51C-ED89093F4A21}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2478D80-0150-4198-8409-D7C527C09EF2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BECCAE-3011-4E47-9C85-DAF9A9A66B8A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D382B29-9896-4F61-9B42-BB255E2E7469}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88169F0E-0699-4038-84DF-A6E784DDA7AD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D0DCCAE-5C79-4A21-8212-5AF36CAB0695}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF13694-BF2E-4CF4-980F-9E02925988CA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20188005-DEAA-4DC4-AB2C-1ED0DA81B40C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B354A5E-B45B-48F8-AE4F-57E49F71FA98}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8303EA-B977-4CF0-B2EF-DFB006C678BA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF53EF4-60F0-4FF8-8692-B3710AD03A83}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE96FF0-466B-4F8B-A108-FDFB7801B3A2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B4D562-C605-4C05-9DAE-55648FE5FE12}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FD1836-148B-4E8C-86CB-F43FB1842DF2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68592F29-CA94-4E1B-8670-3B85437C6AC7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E528FAD3-190B-4BA0-B1D4-9CB05E6FC503}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855F5B9C-41AB-4E27-9999-F7F95BB09D25}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CA8A5A-76CE-4666-8BDE-C8B2371ED3C5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1F0CB4-D2A6-4F1F-B71C-6B8C281DE15D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F837FD77-91F7-489E-BFF5-EA32669C2226}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB687E6F-477A-47AD-A58E-074987329DB6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0CD35B-D50D-450C-B72A-CC1947BDED9E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBFABD8-1D55-4667-8313-EDB797C0D36C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C8388E-04A1-47F6-ABB8-D2B2005A7A73}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{102D6A31-68B2-4591-87D7-ED1B3E566C4F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450D99F8-ECAB-4F56-8433-70C2205EA6C5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A208E9-76BE-4A92-8973-9A35DABB2882}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF1DC09-B0B6-433D-90AA-64488A248DDF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B55635E-6A8D-4A6F-8C34-4DC55504B32F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D696699-4D1D-48A7-9A20-C4BCC2A05349}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9719E2-68D5-48A6-99A9-614439461ECB}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3300,7 +4839,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B72D84A-3CBF-48CB-9EE6-18B3970BD7B3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08E154E-B56F-47B7-8A46-D71CDBFA70D7}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3312,7 +4863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCAB8C6-B2ED-4067-8C9D-DCDA95A6AE86}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3324,7 +4875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8125B6E5-4673-4EA3-91DB-322B4FC9F63E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3336,31 +4887,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2703BBF-422F-438F-864C-5731D622B879}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197A79FD-0175-47AE-9FD3-F3A7DFD76A4B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D2A1F5-63E0-49E7-98F8-5517C9372485}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3372,182 +4899,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187BB5D5-BBCD-42CE-9B2E-0A23A6F2A427}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF5000D-7831-43BF-96AE-24E695C0F737}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1784A7C-BA31-4DE4-9155-73264A1C0EAD}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66431CAB-3F75-437E-AD51-DC5C61918C3F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD711559-4FF8-4246-A0C0-A85B7233DDFD}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D323B320-A9CE-4C67-B48A-94181AF79AE7}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24896845-7777-4C75-BD5B-F58E23B87A70}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24BB7E6-5CEC-493A-969D-B451582ECD09}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05423DF6-3648-48B5-AA83-3CB741922492}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70015B36-DE30-4DC5-A16D-C45E75C14A45}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381CF41D-FEF4-42F3-995D-AC658A3060CE}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DEBD89-A3E0-450C-9D27-C287992B4E3E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CADEA8-3CDB-4730-90A7-153FD37718F0}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C3216E-3A4C-4CAE-94D8-B397A602CC7C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AMJ51"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="144" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="C2" zoomScale="144" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -3569,7 +4928,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="126" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="126"/>
       <c r="C1" s="126"/>
@@ -3587,34 +4946,34 @@
         <v>33</v>
       </c>
       <c r="B3" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="D3" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="E3" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="74" t="s">
+      <c r="F3" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="74" t="s">
+      <c r="G3" s="74" t="s">
         <v>123</v>
       </c>
-      <c r="G3" s="74" t="s">
+      <c r="H3" s="74" t="s">
         <v>124</v>
       </c>
-      <c r="H3" s="74" t="s">
+      <c r="I3" s="75" t="s">
         <v>125</v>
       </c>
-      <c r="I3" s="75" t="s">
+      <c r="J3" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="J3" s="74" t="s">
+      <c r="K3" s="74" t="s">
         <v>127</v>
-      </c>
-      <c r="K3" s="74" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3623,7 +4982,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="77" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C4" s="78" t="s">
         <v>6</v>
@@ -3632,13 +4991,13 @@
         <v>45170</v>
       </c>
       <c r="E4" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="78" t="s">
         <v>130</v>
       </c>
-      <c r="F4" s="78" t="s">
+      <c r="G4" s="78" t="s">
         <v>131</v>
-      </c>
-      <c r="G4" s="78" t="s">
-        <v>132</v>
       </c>
       <c r="H4" s="78" t="s">
         <v>6</v>
@@ -3655,7 +5014,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="82" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" s="83" t="s">
         <v>6</v>
@@ -3664,13 +5023,13 @@
         <v>45170</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="83" t="s">
         <v>133</v>
       </c>
-      <c r="F5" s="83" t="s">
-        <v>134</v>
-      </c>
       <c r="G5" s="83" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H5" s="83" t="s">
         <v>6</v>
@@ -3687,7 +5046,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="82" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C6" s="83" t="s">
         <v>6</v>
@@ -3696,13 +5055,13 @@
         <v>45170</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="83" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" s="83" t="s">
         <v>136</v>
-      </c>
-      <c r="F6" s="83" t="s">
-        <v>134</v>
-      </c>
-      <c r="G6" s="83" t="s">
-        <v>137</v>
       </c>
       <c r="H6" s="83" t="s">
         <v>6</v>
@@ -4167,40 +5526,40 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="F38" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="G38" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G39" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -4221,7 +5580,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4245,7 +5604,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="123" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B1" s="123"/>
       <c r="C1" s="123"/>
@@ -4263,25 +5622,25 @@
         <v>33</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" s="26" t="s">
+      <c r="E3" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="F3" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="G3" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="H3" s="26" t="s">
         <v>149</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -4289,7 +5648,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" s="41">
         <v>4</v>
@@ -4303,7 +5662,7 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -4312,7 +5671,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="41">
         <v>1</v>
@@ -4326,7 +5685,7 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -4335,7 +5694,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C6" s="41">
         <v>2</v>
@@ -4349,7 +5708,7 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -4780,7 +6139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
@@ -4799,134 +6158,134 @@
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="96" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="97" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="98" t="s">
         <v>160</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="C4" s="98" t="s">
         <v>161</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="D4" s="98" t="s">
         <v>162</v>
-      </c>
-      <c r="D4" s="98" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="99" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="100" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="C5" s="100" t="s">
         <v>165</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="D5" s="100" t="s">
         <v>166</v>
-      </c>
-      <c r="D5" s="100" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="100" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="100" t="s">
+      <c r="C6" s="100" t="s">
         <v>169</v>
       </c>
-      <c r="C6" s="100" t="s">
+      <c r="D6" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="K6" s="101" t="s">
         <v>170</v>
-      </c>
-      <c r="D6" s="100" t="s">
-        <v>167</v>
-      </c>
-      <c r="K6" s="101" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="99" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="B7" s="100" t="s">
+      <c r="C7" s="100" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="100" t="s">
         <v>173</v>
       </c>
-      <c r="C7" s="100" t="s">
-        <v>170</v>
-      </c>
-      <c r="D7" s="100" t="s">
+      <c r="K7" s="97" t="s">
         <v>174</v>
       </c>
-      <c r="K7" s="97" t="s">
+      <c r="L7" s="97" t="s">
         <v>175</v>
       </c>
-      <c r="L7" s="97" t="s">
+      <c r="M7" s="97" t="s">
         <v>176</v>
       </c>
-      <c r="M7" s="97" t="s">
+      <c r="N7" s="97" t="s">
         <v>177</v>
-      </c>
-      <c r="N7" s="97" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="99" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" s="100" t="s">
         <v>179</v>
       </c>
-      <c r="B8" s="100" t="s">
+      <c r="C8" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="100" t="s">
         <v>180</v>
       </c>
-      <c r="C8" s="100" t="s">
-        <v>167</v>
-      </c>
-      <c r="D8" s="100" t="s">
+      <c r="K8" s="99" t="s">
+        <v>172</v>
+      </c>
+      <c r="L8" s="99" t="s">
+        <v>166</v>
+      </c>
+      <c r="M8" s="99" t="s">
+        <v>166</v>
+      </c>
+      <c r="N8" s="99" t="s">
         <v>181</v>
-      </c>
-      <c r="K8" s="99" t="s">
-        <v>173</v>
-      </c>
-      <c r="L8" s="99" t="s">
-        <v>167</v>
-      </c>
-      <c r="M8" s="99" t="s">
-        <v>167</v>
-      </c>
-      <c r="N8" s="99" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="99" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B9" s="100"/>
       <c r="C9" s="100"/>
       <c r="D9" s="100"/>
       <c r="K9" s="99" t="s">
+        <v>172</v>
+      </c>
+      <c r="L9" s="99" t="s">
+        <v>166</v>
+      </c>
+      <c r="M9" s="99" t="s">
         <v>173</v>
       </c>
-      <c r="L9" s="99" t="s">
-        <v>167</v>
-      </c>
-      <c r="M9" s="99" t="s">
-        <v>174</v>
-      </c>
       <c r="N9" s="99" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -4935,16 +6294,16 @@
       <c r="C10" s="100"/>
       <c r="D10" s="100"/>
       <c r="K10" s="99" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L10" s="99" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M10" s="99" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N10" s="99" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -4953,16 +6312,16 @@
       <c r="C11" s="100"/>
       <c r="D11" s="100"/>
       <c r="K11" s="99" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L11" s="99" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M11" s="99" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N11" s="99" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -4971,16 +6330,16 @@
       <c r="C12" s="100"/>
       <c r="D12" s="100"/>
       <c r="K12" s="99" t="s">
+        <v>172</v>
+      </c>
+      <c r="L12" s="99" t="s">
         <v>173</v>
-      </c>
-      <c r="L12" s="99" t="s">
-        <v>174</v>
       </c>
       <c r="M12" s="99" t="s">
         <v>47</v>
       </c>
       <c r="N12" s="99" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -5027,40 +6386,40 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="97" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B21" s="128" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C21" s="128"/>
       <c r="D21" s="128"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="102" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B22" s="129" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C22" s="129"/>
       <c r="D22" s="129"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="102" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="129" t="s">
         <v>190</v>
-      </c>
-      <c r="B23" s="129" t="s">
-        <v>191</v>
       </c>
       <c r="C23" s="129"/>
       <c r="D23" s="129"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="102" t="s">
+        <v>191</v>
+      </c>
+      <c r="B24" s="129" t="s">
         <v>192</v>
-      </c>
-      <c r="B24" s="129" t="s">
-        <v>193</v>
       </c>
       <c r="C24" s="129"/>
       <c r="D24" s="129"/>
@@ -5123,15 +6482,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="112" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="111" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5144,20 +6503,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="123" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="B1" s="123"/>
       <c r="C1" s="123"/>
     </row>
     <row r="3" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="C3" s="26" t="s">
         <v>195</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -5168,7 +6527,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5179,7 +6538,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -5190,7 +6549,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -5201,7 +6560,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -5212,7 +6571,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
@@ -5223,28 +6582,52 @@
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="2"/>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="288" x14ac:dyDescent="0.3">
+      <c r="A10" s="40">
+        <v>45271</v>
+      </c>
+      <c r="B10" s="41">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="40">
+        <v>45278</v>
+      </c>
+      <c r="B11" s="41">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A12" s="40">
+        <v>45299</v>
+      </c>
+      <c r="B12" s="41">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="40">
+        <v>45306</v>
+      </c>
+      <c r="B13" s="41">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
@@ -5355,7 +6738,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
@@ -5372,26 +6755,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="105" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="105" t="s">
         <v>198</v>
-      </c>
-      <c r="B1" s="105" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="104" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="104" t="s">
         <v>200</v>
-      </c>
-      <c r="B2" s="104" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="104" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" s="104" t="s">
         <v>202</v>
-      </c>
-      <c r="B3" s="104" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -5400,8 +6783,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2508AE-0669-4824-9D00-E9F459DA123E}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993C6B61-CEF1-423C-A4E7-CE807CAC6669}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5412,8 +6795,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908C48C1-53E0-4CCE-8001-792C04797C32}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33A0ACE-6F9F-40A9-AA45-3C2CA89EEFFF}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5424,8 +6807,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C6D575-2F4C-4332-831A-F80F06F29E06}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645B3D95-2DBE-48D2-8A4B-53776C03C6B6}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5434,839 +6817,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:D26"/>
-  <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="84" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="7.109375" customWidth="1"/>
-    <col min="2" max="2" width="58.88671875" style="25" customWidth="1"/>
-    <col min="3" max="3" width="39.5546875" style="25" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="64" width="10.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="118" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-    </row>
-    <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="122" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="122"/>
-    </row>
-    <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="122" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="122"/>
-    </row>
-    <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="122" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="122"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="28">
-        <v>10</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="30"/>
-    </row>
-    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="28">
-        <v>20</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>206</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>207</v>
-      </c>
-      <c r="D10" s="30"/>
-    </row>
-    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="28">
-        <v>30</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>208</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="30"/>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="28">
-        <v>40</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="30"/>
-    </row>
-    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="28">
-        <v>51</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="30"/>
-    </row>
-    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="28">
-        <v>52</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="30"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="28">
-        <v>60</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="30"/>
-    </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="28">
-        <v>61</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="30"/>
-    </row>
-    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="28">
-        <v>62</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="30"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="28">
-        <v>50</v>
-      </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="28">
-        <v>60</v>
-      </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="31"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="28">
-        <v>70</v>
-      </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="28">
-        <v>80</v>
-      </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="28">
-        <v>90</v>
-      </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="28">
-        <v>100</v>
-      </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="32">
-        <v>110</v>
-      </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:C41"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="114" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="56.44140625" customWidth="1"/>
-    <col min="2" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="64" width="10.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="123" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="23"/>
-    </row>
-    <row r="3" spans="1:3" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="124" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-    </row>
-    <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="125" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="125"/>
-      <c r="C4" s="125"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="23"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="37">
-        <v>45236</v>
-      </c>
-      <c r="C7" s="37">
-        <v>45236</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="39">
-        <v>45243</v>
-      </c>
-      <c r="C8" s="39"/>
-    </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="38" t="s">
-        <v>209</v>
-      </c>
-      <c r="B9" s="39">
-        <v>45257</v>
-      </c>
-      <c r="C9" s="39"/>
-    </row>
-    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="40">
-        <v>45271</v>
-      </c>
-      <c r="C10" s="41"/>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="39">
-        <v>45278</v>
-      </c>
-      <c r="C11" s="41"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="39">
-        <v>45306</v>
-      </c>
-      <c r="C12" s="41"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="39">
-        <v>45320</v>
-      </c>
-      <c r="C13" s="41"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="39">
-        <v>45341</v>
-      </c>
-      <c r="C14" s="41"/>
-    </row>
-    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" s="39">
-        <v>45355</v>
-      </c>
-      <c r="C15" s="41"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="39">
-        <v>45362</v>
-      </c>
-      <c r="C16" s="41"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="40"/>
-      <c r="C18" s="41"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="41"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="24"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:AMJ21"/>
-  <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3.44140625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="43.88671875" style="23" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" style="35" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="23" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="23" customWidth="1"/>
-    <col min="6" max="6" width="68.6640625" style="23" customWidth="1"/>
-    <col min="7" max="1024" width="11.44140625" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="123" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-    </row>
-    <row r="3" spans="1:6" s="43" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="41">
-        <v>1</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="41">
-        <v>1</v>
-      </c>
-      <c r="D4" s="44">
-        <v>50</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="45" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="41">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="41">
-        <v>2</v>
-      </c>
-      <c r="D5" s="44">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="45" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="41">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="41">
-        <v>1</v>
-      </c>
-      <c r="D6" s="44">
-        <v>2.5</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="45"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="41">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="41">
-        <v>1</v>
-      </c>
-      <c r="D7" s="44">
-        <v>2</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="41">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="44">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="41">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="41">
-        <v>1</v>
-      </c>
-      <c r="D9" s="44">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="41">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="41">
-        <v>1</v>
-      </c>
-      <c r="D10" s="44">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="41">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="41">
-        <v>3</v>
-      </c>
-      <c r="D11" s="44">
-        <v>45</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="46"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="41">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="41">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="41">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="41">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="41">
-        <v>26</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="41">
-        <v>27</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="41">
-        <v>28</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="41">
-        <v>29</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="42">
-        <v>30</v>
-      </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-    </row>
-    <row r="21" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="47"/>
-      <c r="B21" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="47"/>
-      <c r="D21" s="48">
-        <f>SUM(D4:D20)</f>
-        <v>121.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="F5" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
 </file>
</xml_diff>